<commit_message>
new testdata in excel
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
   <si>
     <t>i1.png</t>
   </si>
@@ -124,12 +124,39 @@
   </si>
   <si>
     <t>K2*LOG(P2)</t>
+  </si>
+  <si>
+    <t>y24.png</t>
+  </si>
+  <si>
+    <t>y25.png</t>
+  </si>
+  <si>
+    <t>Z27.png</t>
+  </si>
+  <si>
+    <t>j29.png</t>
+  </si>
+  <si>
+    <t>j30.png</t>
+  </si>
+  <si>
+    <t>k31.png</t>
+  </si>
+  <si>
+    <t>k32.png</t>
+  </si>
+  <si>
+    <t>j33.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="#,##0.000000000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,12 +186,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -382,11 +417,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="538979136"/>
-        <c:axId val="529543680"/>
+        <c:axId val="90151680"/>
+        <c:axId val="90152256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="538979136"/>
+        <c:axId val="90151680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,12 +432,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="529543680"/>
+        <c:crossAx val="90152256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="529543680"/>
+        <c:axId val="90152256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,7 +447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="538979136"/>
+        <c:crossAx val="90151680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -596,11 +631,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="545681920"/>
-        <c:axId val="539039360"/>
+        <c:axId val="101367808"/>
+        <c:axId val="101368384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="545681920"/>
+        <c:axId val="101367808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,12 +645,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539039360"/>
+        <c:crossAx val="101368384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="539039360"/>
+        <c:axId val="101368384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,7 +661,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="545681920"/>
+        <c:crossAx val="101367808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -977,7 +1012,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -985,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q149"/>
+  <dimension ref="A1:AA149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,14 +1031,21 @@
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="12" width="11.42578125" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" customWidth="1"/>
     <col min="15" max="15" width="11.7109375" customWidth="1"/>
     <col min="17" max="17" width="22.28515625" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" customWidth="1"/>
+    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" customWidth="1"/>
+    <col min="27" max="27" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:27" x14ac:dyDescent="0.25">
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1032,8 +1074,30 @@
       <c r="Q1" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1060,11 +1124,30 @@
         <v>9184</v>
       </c>
       <c r="Q2">
-        <f>K2*LOG(P2)</f>
+        <f t="shared" ref="Q2:Q26" si="0">K2*LOG(P2)</f>
         <v>4755.6382500646778</v>
       </c>
-    </row>
-    <row r="3" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U2" s="2">
+        <v>74</v>
+      </c>
+      <c r="V2" s="2">
+        <v>1246</v>
+      </c>
+      <c r="W2" s="2"/>
+      <c r="X2" s="5">
+        <v>842.31859999999995</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="3" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1075,7 +1158,7 @@
         <v>12164</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" ref="L3:L26" si="0">K3*M3</f>
+        <f t="shared" ref="L3:L26" si="1">K3*M3</f>
         <v>9220312</v>
       </c>
       <c r="M3" s="2">
@@ -1091,11 +1174,30 @@
         <v>96270</v>
       </c>
       <c r="Q3">
-        <f>K3*LOG(P3)</f>
+        <f t="shared" si="0"/>
         <v>60619.18418115969</v>
       </c>
-    </row>
-    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" s="2">
+        <v>596</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" s="2"/>
+      <c r="X3" s="6">
+        <v>521.66079999999999</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="4" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1106,7 +1208,7 @@
         <v>17556</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2668512</v>
       </c>
       <c r="M4" s="2">
@@ -1122,11 +1224,30 @@
         <v>140448</v>
       </c>
       <c r="Q4">
-        <f>K4*LOG(P4)</f>
+        <f t="shared" si="0"/>
         <v>90369.783156698613</v>
       </c>
-    </row>
-    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U4" s="2">
+        <v>40</v>
+      </c>
+      <c r="V4" s="2">
+        <v>656</v>
+      </c>
+      <c r="W4" s="2"/>
+      <c r="X4" s="5">
+        <v>570.77229999999997</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="5" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1137,7 +1258,7 @@
         <v>1200</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48000</v>
       </c>
       <c r="M5" s="2">
@@ -1153,11 +1274,30 @@
         <v>9184</v>
       </c>
       <c r="Q5">
-        <f>K5*LOG(P5)</f>
+        <f t="shared" si="0"/>
         <v>4755.6382500646778</v>
       </c>
-    </row>
-    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="2">
+        <v>1149</v>
+      </c>
+      <c r="U5" s="2">
+        <v>108</v>
+      </c>
+      <c r="V5" s="2">
+        <v>1596</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="X5" s="5">
+        <v>423.49860000000001</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>8827</v>
+      </c>
+    </row>
+    <row r="6" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1168,7 +1308,7 @@
         <v>596</v>
       </c>
       <c r="L6" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -1184,11 +1324,30 @@
         <v>4566</v>
       </c>
       <c r="Q6">
-        <f>K6*LOG(P6)</f>
+        <f t="shared" si="0"/>
         <v>2181.0834006639129</v>
       </c>
-    </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T6" s="2">
+        <v>360</v>
+      </c>
+      <c r="U6" s="2">
+        <v>32</v>
+      </c>
+      <c r="V6" s="2">
+        <v>348</v>
+      </c>
+      <c r="W6" s="2"/>
+      <c r="X6" s="6">
+        <v>255.72929999999999</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>2826</v>
+      </c>
+    </row>
+    <row r="7" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1199,7 +1358,7 @@
         <v>1149</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>124092</v>
       </c>
       <c r="M7" s="2">
@@ -1215,11 +1374,30 @@
         <v>8827</v>
       </c>
       <c r="Q7">
-        <f>K7*LOG(P7)</f>
+        <f t="shared" si="0"/>
         <v>4533.7392824488525</v>
       </c>
-    </row>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" s="2">
+        <v>239</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="X7" s="5">
+        <v>359.44549999999998</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="8" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1230,7 +1408,7 @@
         <v>239</v>
       </c>
       <c r="L8" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -1246,11 +1424,30 @@
         <v>1832</v>
       </c>
       <c r="Q8">
-        <f>K8*LOG(P8)</f>
+        <f t="shared" si="0"/>
         <v>779.83918717030781</v>
       </c>
-    </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U8" s="2">
+        <v>54</v>
+      </c>
+      <c r="V8" s="2">
+        <v>982</v>
+      </c>
+      <c r="W8" s="2"/>
+      <c r="X8" s="5">
+        <v>419.12189999999998</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="9" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1261,7 +1458,7 @@
         <v>4365</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>397215</v>
       </c>
       <c r="M9" s="2">
@@ -1277,11 +1474,30 @@
         <v>34090</v>
       </c>
       <c r="Q9">
-        <f>K9*LOG(P9)</f>
+        <f t="shared" si="0"/>
         <v>19784.916860364112</v>
       </c>
-    </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9" s="2">
+        <v>767</v>
+      </c>
+      <c r="U9" s="2">
+        <v>27</v>
+      </c>
+      <c r="V9" s="2">
+        <v>380</v>
+      </c>
+      <c r="W9" s="2"/>
+      <c r="X9" s="5">
+        <v>361.92089999999899</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>5936</v>
+      </c>
+    </row>
+    <row r="10" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1292,7 +1508,7 @@
         <v>360</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11520</v>
       </c>
       <c r="M10" s="2">
@@ -1308,11 +1524,30 @@
         <v>2826</v>
       </c>
       <c r="Q10">
-        <f>K10*LOG(P10)</f>
+        <f t="shared" si="0"/>
         <v>1242.4219767045145</v>
       </c>
-    </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T10" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U10" s="2">
+        <v>78</v>
+      </c>
+      <c r="V10" s="2">
+        <v>912</v>
+      </c>
+      <c r="W10" s="2"/>
+      <c r="X10" s="5">
+        <v>428.93180000000001</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="11" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1323,7 +1558,7 @@
         <v>239</v>
       </c>
       <c r="L11" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -1339,11 +1574,30 @@
         <v>1832</v>
       </c>
       <c r="Q11">
-        <f>K11*LOG(P11)</f>
+        <f t="shared" si="0"/>
         <v>779.83918717030781</v>
       </c>
-    </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T11" s="2">
+        <v>1190</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W11" s="2"/>
+      <c r="X11" s="5">
+        <v>444.83949999999902</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>9131</v>
+      </c>
+    </row>
+    <row r="12" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1354,7 +1608,7 @@
         <v>1200</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64800</v>
       </c>
       <c r="M12" s="2">
@@ -1370,11 +1624,30 @@
         <v>9184</v>
       </c>
       <c r="Q12">
-        <f>K12*LOG(P12)</f>
+        <f t="shared" si="0"/>
         <v>4755.6382500646778</v>
       </c>
-    </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U12" s="2">
+        <v>52</v>
+      </c>
+      <c r="V12" s="2">
+        <v>600</v>
+      </c>
+      <c r="W12" s="2"/>
+      <c r="X12" s="5">
+        <v>558.33590000000004</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="13" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1385,7 +1658,7 @@
         <v>1200</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>268800</v>
       </c>
       <c r="M13" s="2">
@@ -1401,11 +1674,30 @@
         <v>9184</v>
       </c>
       <c r="Q13">
-        <f>K13*LOG(P13)</f>
+        <f t="shared" si="0"/>
         <v>4755.6382500646778</v>
       </c>
-    </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T13" s="2">
+        <v>600</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W13" s="2"/>
+      <c r="X13" s="5">
+        <v>355.76299999999998</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>4592</v>
+      </c>
+    </row>
+    <row r="14" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1416,7 +1708,7 @@
         <v>767</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20709</v>
       </c>
       <c r="M14" s="2">
@@ -1432,11 +1724,30 @@
         <v>5936</v>
       </c>
       <c r="Q14">
-        <f>K14*LOG(P14)</f>
+        <f t="shared" si="0"/>
         <v>2894.2698153718343</v>
       </c>
-    </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U14" s="2">
+        <v>224</v>
+      </c>
+      <c r="V14" s="2">
+        <v>2292</v>
+      </c>
+      <c r="W14" s="2"/>
+      <c r="X14" s="5">
+        <v>596.09088888888903</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="15" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1447,7 +1758,7 @@
         <v>1200</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>93600</v>
       </c>
       <c r="M15" s="2">
@@ -1463,11 +1774,31 @@
         <v>9184</v>
       </c>
       <c r="Q15">
-        <f>K15*LOG(P15)</f>
+        <f t="shared" si="0"/>
         <v>4755.6382500646778</v>
       </c>
-    </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T15" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U15" s="2">
+        <v>22</v>
+      </c>
+      <c r="V15" s="2">
+        <v>320</v>
+      </c>
+      <c r="W15" s="2"/>
+      <c r="X15" s="5">
+        <v>458.57389999999998</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>9184</v>
+      </c>
+      <c r="AA15" s="4"/>
+    </row>
+    <row r="16" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1478,7 +1809,7 @@
         <v>1190</v>
       </c>
       <c r="L16" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M16" s="2" t="s">
@@ -1494,11 +1825,30 @@
         <v>9131</v>
       </c>
       <c r="Q16">
-        <f>K16*LOG(P16)</f>
+        <f t="shared" si="0"/>
         <v>4713.0168279090421</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T16" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U16" s="2">
+        <v>34</v>
+      </c>
+      <c r="V16" s="2">
+        <v>376</v>
+      </c>
+      <c r="W16" s="2"/>
+      <c r="X16" s="6">
+        <v>457.09449999999998</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1509,7 +1859,7 @@
         <v>1200</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62400</v>
       </c>
       <c r="M17" s="2">
@@ -1525,11 +1875,30 @@
         <v>9184</v>
       </c>
       <c r="Q17">
-        <f>K17*LOG(P17)</f>
+        <f t="shared" si="0"/>
         <v>4755.6382500646778</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T17" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U17" s="2">
+        <v>38</v>
+      </c>
+      <c r="V17" s="2">
+        <v>760</v>
+      </c>
+      <c r="W17" s="2"/>
+      <c r="X17" s="5">
+        <v>523.26089999999999</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1540,7 +1909,7 @@
         <v>600</v>
       </c>
       <c r="L18" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -1556,11 +1925,30 @@
         <v>4592</v>
       </c>
       <c r="Q18">
-        <f>K18*LOG(P18)</f>
+        <f t="shared" si="0"/>
         <v>2197.2011276339504</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T18" s="2">
+        <v>1146</v>
+      </c>
+      <c r="U18" s="2">
+        <v>178</v>
+      </c>
+      <c r="V18" s="2">
+        <v>1928</v>
+      </c>
+      <c r="W18" s="2"/>
+      <c r="X18" s="5">
+        <v>435.27100000000002</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>8826</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1571,7 +1959,7 @@
         <v>1200</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26400</v>
       </c>
       <c r="M19" s="2">
@@ -1587,11 +1975,30 @@
         <v>9184</v>
       </c>
       <c r="Q19">
-        <f>K19*LOG(P19)</f>
+        <f t="shared" si="0"/>
         <v>4755.6382500646778</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T19" s="2">
+        <v>1137</v>
+      </c>
+      <c r="U19" s="2">
+        <v>41</v>
+      </c>
+      <c r="V19" s="2">
+        <v>690</v>
+      </c>
+      <c r="W19" s="2"/>
+      <c r="X19" s="5">
+        <v>635.15729999999996</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>8722</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1602,7 +2009,7 @@
         <v>1200</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40800</v>
       </c>
       <c r="M20" s="2">
@@ -1618,11 +2025,30 @@
         <v>9184</v>
       </c>
       <c r="Q20">
-        <f>K20*LOG(P20)</f>
+        <f t="shared" si="0"/>
         <v>4755.6382500646778</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T20" s="2">
+        <v>1028</v>
+      </c>
+      <c r="U20" s="2">
+        <v>187</v>
+      </c>
+      <c r="V20" s="2">
+        <v>2486</v>
+      </c>
+      <c r="W20" s="2"/>
+      <c r="X20" s="6">
+        <v>497.421999999999</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>7944</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1633,7 +2059,7 @@
         <v>1137</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46617</v>
       </c>
       <c r="M21" s="2">
@@ -1649,11 +2075,30 @@
         <v>8722</v>
       </c>
       <c r="Q21">
-        <f>K21*LOG(P21)</f>
+        <f t="shared" si="0"/>
         <v>4480.4804856176324</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T21" s="2">
+        <v>832</v>
+      </c>
+      <c r="U21" s="2">
+        <v>53</v>
+      </c>
+      <c r="V21" s="2">
+        <v>792</v>
+      </c>
+      <c r="W21" s="2"/>
+      <c r="X21" s="5">
+        <v>497.6035</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>6329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1664,7 +2109,7 @@
         <v>1028</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>192236</v>
       </c>
       <c r="M22" s="2">
@@ -1680,11 +2125,30 @@
         <v>7944</v>
       </c>
       <c r="Q22">
-        <f>K22*LOG(P22)</f>
+        <f t="shared" si="0"/>
         <v>4009.2403340809697</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T22" s="2">
+        <v>629</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W22" s="2"/>
+      <c r="X22" s="5">
+        <v>427.22133300000002</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>4830</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1695,7 +2159,7 @@
         <v>832</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44096</v>
       </c>
       <c r="M23" s="2">
@@ -1711,11 +2175,30 @@
         <v>6329</v>
       </c>
       <c r="Q23">
-        <f>K23*LOG(P23)</f>
+        <f t="shared" si="0"/>
         <v>3162.7107996012228</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23" s="2">
+        <v>4365</v>
+      </c>
+      <c r="U23" s="2">
+        <v>91</v>
+      </c>
+      <c r="V23" s="2">
+        <v>1202</v>
+      </c>
+      <c r="W23" s="2"/>
+      <c r="X23" s="5">
+        <v>2242.6107000000002</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>34090</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1726,7 +2209,7 @@
         <v>629</v>
       </c>
       <c r="L24" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M24" s="2" t="s">
@@ -1742,11 +2225,30 @@
         <v>4830</v>
       </c>
       <c r="Q24">
-        <f>K24*LOG(P24)</f>
+        <f t="shared" si="0"/>
         <v>2317.202745242701</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T24" s="2">
+        <v>239</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W24" s="2"/>
+      <c r="X24" s="5">
+        <v>753.54389999999898</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1757,7 +2259,7 @@
         <v>1200</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45600</v>
       </c>
       <c r="M25" s="2">
@@ -1773,11 +2275,30 @@
         <v>9184</v>
       </c>
       <c r="Q25">
-        <f>K25*LOG(P25)</f>
+        <f t="shared" si="0"/>
         <v>4755.6382500646778</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T25" s="2">
+        <v>2330</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W25" s="2"/>
+      <c r="X25" s="5">
+        <v>1651.0107</v>
+      </c>
+      <c r="Y25" s="2">
+        <v>18228</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="D26" s="1"/>
       <c r="F26" s="2"/>
@@ -1789,7 +2310,7 @@
         <v>1146</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>203988</v>
       </c>
       <c r="M26" s="2">
@@ -1805,170 +2326,373 @@
         <v>8826</v>
       </c>
       <c r="Q26">
-        <f>K26*LOG(P26)</f>
+        <f t="shared" si="0"/>
         <v>4521.8454558854046</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T26" s="2">
+        <v>2924</v>
+      </c>
+      <c r="U26" s="2">
+        <v>54</v>
+      </c>
+      <c r="V26" s="2">
+        <v>772</v>
+      </c>
+      <c r="W26" s="2"/>
+      <c r="X26" s="5">
+        <v>1781.2599</v>
+      </c>
+      <c r="Y26" s="2">
+        <v>23056</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T27" s="2">
+        <v>12164</v>
+      </c>
+      <c r="U27" s="2">
+        <v>758</v>
+      </c>
+      <c r="V27" s="2">
+        <v>9946</v>
+      </c>
+      <c r="W27" s="2"/>
+      <c r="X27" s="5">
+        <v>8199.0594000000001</v>
+      </c>
+      <c r="Y27" s="2">
+        <v>96270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T28" s="2">
+        <v>19124</v>
+      </c>
+      <c r="U28" s="2">
+        <v>165</v>
+      </c>
+      <c r="V28" s="2">
+        <v>2726</v>
+      </c>
+      <c r="W28" s="2"/>
+      <c r="X28" s="6">
+        <v>12324.140799999999</v>
+      </c>
+      <c r="Y28" s="2">
+        <v>151316</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T29" s="2">
+        <v>17556</v>
+      </c>
+      <c r="U29" s="2">
+        <v>152</v>
+      </c>
+      <c r="V29" s="2">
+        <v>3082</v>
+      </c>
+      <c r="W29" s="2"/>
+      <c r="X29" s="5">
+        <v>13721.957899999999</v>
+      </c>
+      <c r="Y29" s="2">
+        <v>140448</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T30" s="2">
+        <v>1322</v>
+      </c>
+      <c r="U30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W30" s="2"/>
+      <c r="X30" s="6">
+        <v>565.06730000000005</v>
+      </c>
+      <c r="Y30" s="2">
+        <v>10281</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T31" s="2">
+        <v>2700</v>
+      </c>
+      <c r="U31" s="2">
+        <v>52</v>
+      </c>
+      <c r="V31" s="2">
+        <v>572</v>
+      </c>
+      <c r="W31" s="2"/>
+      <c r="X31" s="5">
+        <v>811.65049999999906</v>
+      </c>
+      <c r="Y31" s="2">
+        <v>20974</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="S32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T32" s="2">
+        <v>10529</v>
+      </c>
+      <c r="U32" s="2">
+        <v>61</v>
+      </c>
+      <c r="V32" s="2">
+        <v>1082</v>
+      </c>
+      <c r="W32" s="2"/>
+      <c r="X32" s="5">
+        <v>4534.6043</v>
+      </c>
+      <c r="Y32" s="2">
+        <v>83009</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="S33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T33" s="2">
+        <v>9985</v>
+      </c>
+      <c r="U33" s="2">
+        <v>227</v>
+      </c>
+      <c r="V33" s="2">
+        <v>3728</v>
+      </c>
+      <c r="W33" s="2"/>
+      <c r="X33" s="6">
+        <v>4899.0306</v>
+      </c>
+      <c r="Y33" s="2">
+        <v>78666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="S34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T34" s="2">
+        <v>2699</v>
+      </c>
+      <c r="U34" s="2">
+        <v>117</v>
+      </c>
+      <c r="V34" s="2">
+        <v>1376</v>
+      </c>
+      <c r="W34" s="2"/>
+      <c r="X34" s="5">
+        <v>1235.2694999999901</v>
+      </c>
+      <c r="Y34" s="2">
+        <v>20966</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X36" s="3"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X37" s="3"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X38" s="3"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X39" s="3"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X40" s="3"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X41" s="3"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X42" s="3"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X43" s="3"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X47" s="3"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X48" s="3"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X49" s="3"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X50" s="3"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X51" s="3"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X52" s="3"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X53" s="3"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X54" s="3"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X55" s="3"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X59" s="3"/>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X60" s="3"/>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X61" s="3"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X62" s="3"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X63" s="3"/>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X64" s="3"/>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X65" s="3"/>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X69" s="3"/>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X71" s="3"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X73" s="3"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X74" s="3"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X75" s="3"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X76" s="3"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X77" s="3"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="X78" s="3"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>